<commit_message>
Removing and rerunning all the appendix tables
</commit_message>
<xml_diff>
--- a/results/tableA1_panel_any_evidence.xlsx
+++ b/results/tableA1_panel_any_evidence.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>eq_mix</t>
   </si>
@@ -43,46 +43,43 @@
     <t>['hour']</t>
   </si>
   <si>
-    <t>(0.44)</t>
-  </si>
-  <si>
-    <t>(0.42)</t>
+    <t>(0.37)</t>
+  </si>
+  <si>
+    <t>(0.22)</t>
   </si>
   <si>
     <t>['year', 'hour']</t>
   </si>
   <si>
-    <t>(0.08)</t>
-  </si>
-  <si>
-    <t>(0.09)</t>
+    <t>(0.18)</t>
+  </si>
+  <si>
+    <t>(0.14)</t>
   </si>
   <si>
     <t>['year', 'weekend', 'hour']</t>
   </si>
   <si>
-    <t>(0.41)</t>
-  </si>
-  <si>
-    <t>(0.33)</t>
+    <t>(0.2)</t>
+  </si>
+  <si>
+    <t>(0.17)</t>
   </si>
   <si>
     <t>['year', 'state', 'hour']</t>
   </si>
   <si>
-    <t>(0.18)</t>
-  </si>
-  <si>
-    <t>(0.3)</t>
+    <t>(0.26)</t>
+  </si>
+  <si>
+    <t>(0.19)</t>
   </si>
   <si>
     <t>['year', 'state', 'weekend', 'hour']</t>
   </si>
   <si>
-    <t>(0.32)</t>
-  </si>
-  <si>
-    <t>(0.12)</t>
+    <t>(0.28)</t>
   </si>
 </sst>
 </file>
@@ -578,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:7">

</xml_diff>